<commit_message>
[Update] Quest xlsx & csv file
[Update] Quest xlsx & csv file
</commit_message>
<xml_diff>
--- a/Documents/Files/Quest.xlsx
+++ b/Documents/Files/Quest.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Sparta_Coding_Club\TeamProject\TextRPG_TeamProject2nd\TextRPG_TeamProject2nd\Documents\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E57CC7D0-77AD-45D5-BBD9-E8C650146CCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5300D17-F3A9-4277-A12C-906F4505BAB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28695" yWindow="16110" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -455,7 +455,7 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -538,6 +538,9 @@
       <c r="G3" s="1">
         <v>100</v>
       </c>
+      <c r="H3" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
@@ -561,6 +564,9 @@
       <c r="G4" s="1">
         <v>135</v>
       </c>
+      <c r="H4" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
@@ -610,6 +616,9 @@
       <c r="G6" s="1">
         <v>135</v>
       </c>
+      <c r="H6" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
@@ -633,6 +642,9 @@
       <c r="G7" s="1">
         <v>250</v>
       </c>
+      <c r="H7" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
@@ -707,6 +719,9 @@
       </c>
       <c r="G10" s="1">
         <v>2000</v>
+      </c>
+      <c r="H10" s="1">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[Complex] Add SceneEnd & Dodge & Critical
[Complex] Add SceneEnd & Dodge & Critical
</commit_message>
<xml_diff>
--- a/Documents/Files/Quest.xlsx
+++ b/Documents/Files/Quest.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Sparta_Coding_Club\TeamProject\TextRPG_TeamProject2nd\TextRPG_TeamProject2nd\Documents\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5300D17-F3A9-4277-A12C-906F4505BAB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F5DD233-8B41-43E3-B71B-E3E0A03B7F47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33255" yWindow="20115" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -67,10 +67,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>최근 늑대들이 농산물을 먹어치우고 있다는 신고가 다발하고 있어요.\n저희 알선소에서도 적극 지원하고 있지만 해결은 요원하네요.\n부디 손을 거들어주시기를 바라겠습니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>전설의 슬라임?!</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -95,36 +91,31 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>늑대들 중에서는 태양의 사자라고 불리는 개체가 있다고 해요.\n사실인지는 모르겠어요. 근데 뭔가 고상해 보이기는 해요. 흔하지만.\n걔네들이 최근 근처 상단을 습격했다고 하니까 개체 수 좀 줄여주세요.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>당신은 저희 알선소에서 첫 번째 임무를 맞이하고 계십니다.\n그래서 역량을 확인하기 위한 간단한 임무로 구성했어요.\n첫 모험에 행운이 가득하기를 빌겠습니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>그거 아세요? 원래 슬라임은 슬라루의 제왕개체였다고 해요.\n그래서인지 슬라임의 체액이 보약이라는 소문도 도처에 퍼져있구요.\n그딴 거 없는데 말이죠. 괜한 피해자가 나오지 않게 수를 줄여주세요.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>아... 결국에는 민간인이 슬라임한테 돌격하는 사건이 발생해버렸어요.\n엄청 큰 슬라임을 만나서 '전설의 슬라임이다!' 하고 달려들었다네요.\n보고 상으로는 평균 크기 보다 조금 작았습니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>늑대들 중에서는 달의 사자라고 불리는 개체가…\n이건 이전에도 설명 드렸을테니 각설하고.\n이번에는 얘네들이 집단 서리를 했대요. 꽤나 많이 털린 모양인지 농장주 께서 좀 많이 화나셨다고…</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>최근 도시 근처 연못에서 크지는 않은데 뭔가 고급진 슬라임이 등장했다고 해요.\n마찬가지로 '보약 아니냐?!'라는 소문이 계속해서 퍼진다고 하네요.\n슬라임 따위한테 그딴거 없을테니 토벌 해 주세요.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>최근 늑대무리의 이상현상의 원인이 밝혀졌습니다.\n늑대들의 신... 과거의 찬달자... 세계의 구원자…\n그 모독적인 껍데기를 처치해 주세요.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>가도에 엄청 큰 늑대가 발견됬다는 보고가 잇다르고 있어요.\n어차피 모험가들이 자주 다니는 길목이라 놔둬도 되기는 하는데…\n아무래도 사람을 습격한다고 합니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <t>당신은 저희 알선소에서 첫 번째 임무를 맞이하고 계십니다.@그래서 역량을 확인하기 위한 간단한 임무로 구성했어요.@첫 모험에 행운이 가득하기를 빌겠습니다.</t>
+  </si>
+  <si>
+    <t>최근 늑대들이 농산물을 먹어치우고 있다는 신고가 다발하고 있어요.@저희 알선소에서도 적극 지원하고 있지만 해결은 요원하네요.@부디 손을 거들어주시기를 바라겠습니다.</t>
+  </si>
+  <si>
+    <t>그거 아세요? 원래 슬라임은 슬라루의 제왕개체였다고 해요.@그래서인지 슬라임의 체액이 보약이라는 소문도 도처에 퍼져있구요.@그딴 거 없는데 말이죠. 괜한 피해자가 나오지 않게 수를 줄여주세요.</t>
+  </si>
+  <si>
+    <t>아... 결국에는 민간인이 슬라임한테 돌격하는 사건이 발생해버렸어요.@엄청 큰 슬라임을 만나서 '전설의 슬라임이다!' 하고 달려들었다네요.@보고 상으로는 평균 크기 보다 조금 작았습니다.</t>
+  </si>
+  <si>
+    <t>가도에 엄청 큰 늑대가 발견됬다는 보고가 잇다르고 있어요.@어차피 모험가들이 자주 다니는 길목이라 놔둬도 되기는 하는데…@아무래도 사람을 습격한다고 합니다.</t>
+  </si>
+  <si>
+    <t>늑대들 중에서는 태양의 사자라고 불리는 개체가 있다고 해요.@사실인지는 모르겠어요. 근데 뭔가 고상해 보이기는 해요. 흔하지만.@걔네들이 최근 근처 상단을 습격했다고 하니까 개체 수 좀 줄여주세요.</t>
+  </si>
+  <si>
+    <t>늑대들 중에서는 달의 사자라고 불리는 개체가…@이건 이전에도 설명 드렸을테니 각설하고.@이번에는 얘네들이 집단 서리를 했대요. 꽤나 많이 털린 모양인지 농장주 께서 좀 많이 화나셨다고…</t>
+  </si>
+  <si>
+    <t>최근 도시 근처 연못에서 크지는 않은데 뭔가 고급진 슬라임이 등장했다고 해요.@마찬가지로 '보약 아니냐?!'라는 소문이 계속해서 퍼진다고 하네요.@슬라임 따위한테 그딴거 없을테니 토벌 해 주세요.</t>
+  </si>
+  <si>
+    <t>최근 늑대무리의 이상현상의 원인이 밝혀졌습니다.@늑대들의 신... 과거의 찬달자... 세계의 구원자…@그 모독적인 껍데기를 처치해 주세요.</t>
   </si>
 </sst>
 </file>
@@ -455,7 +446,7 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -498,7 +489,7 @@
         <v>8</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D2" s="1">
         <v>0</v>
@@ -524,7 +515,7 @@
         <v>9</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="D3" s="1">
         <v>10</v>
@@ -547,10 +538,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D4" s="1">
         <v>1</v>
@@ -573,10 +564,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D5" s="1">
         <v>2</v>
@@ -599,10 +590,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D6" s="1">
         <v>12</v>
@@ -625,10 +616,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D7" s="1">
         <v>14</v>
@@ -651,10 +642,10 @@
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D8" s="1">
         <v>13</v>
@@ -677,10 +668,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D9" s="1">
         <v>6</v>
@@ -703,10 +694,10 @@
         <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D10" s="1">
         <v>17</v>

</xml_diff>